<commit_message>
CANVIS 20 agost 2024
</commit_message>
<xml_diff>
--- a/VARIABLES/gasNatural_filtrat.xlsx
+++ b/VARIABLES/gasNatural_filtrat.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G68"/>
+  <dimension ref="A1:G54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,2192 +476,1750 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>45497</v>
+        <v>45515</v>
       </c>
       <c r="B2" t="n">
-        <v>2.191</v>
+        <v>2.188</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2,186</t>
+          <t>2,189</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2,196</t>
+          <t>2,255</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2,170</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr"/>
+          <t>2,154</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>181,25K</t>
+        </is>
+      </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>-1,48%</t>
+          <t>2,10%</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>45496</v>
+        <v>45508</v>
       </c>
       <c r="B3" t="n">
-        <v>2.224</v>
+        <v>2.143</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2,279</t>
+          <t>1,950</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2,290</t>
+          <t>2,187</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2,160</t>
+          <t>1,882</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>127,42K</t>
+          <t>947,48K</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>-2,71%</t>
+          <t>8,95%</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>45495</v>
+        <v>45501</v>
       </c>
       <c r="B4" t="n">
-        <v>2.286</v>
+        <v>1.967</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2,145</t>
+          <t>2,016</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2,302</t>
+          <t>2,149</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2,131</t>
+          <t>1,856</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>141,07K</t>
+          <t>709,02K</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>5,59%</t>
+          <t>-1,94%</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>45492</v>
+        <v>45494</v>
       </c>
       <c r="B5" t="n">
-        <v>2.165</v>
+        <v>2.006</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2,128</t>
+          <t>2,104</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2,179</t>
+          <t>2,270</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2,095</t>
+          <t>1,994</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>101,00K</t>
+          <t>429,46K</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>-0,14%</t>
+          <t>-5,73%</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>45491</v>
+        <v>45487</v>
       </c>
       <c r="B6" t="n">
-        <v>2.168</v>
+        <v>2.128</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2,088</t>
+          <t>2,273</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2,172</t>
+          <t>2,285</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2,063</t>
+          <t>2,015</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>147,92K</t>
+          <t>794,39K</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>4,68%</t>
+          <t>-8,63%</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>45490</v>
+        <v>45480</v>
       </c>
       <c r="B7" t="n">
-        <v>2.071</v>
+        <v>2.329</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2,203</t>
+          <t>2,270</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2,224</t>
+          <t>2,448</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2,055</t>
+          <t>2,249</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>187,04K</t>
+          <t>715,94K</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>-6,12%</t>
+          <t>-0,89%</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>45489</v>
+        <v>45473</v>
       </c>
       <c r="B8" t="n">
-        <v>2.206</v>
+        <v>2.35</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2,189</t>
+          <t>2,581</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2,235</t>
+          <t>2,599</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2,171</t>
+          <t>2,347</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>121,32K</t>
+          <t>372,57K</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>1,29%</t>
+          <t>-9,65%</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>45488</v>
+        <v>45466</v>
       </c>
       <c r="B9" t="n">
-        <v>2.178</v>
+        <v>2.601</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2,283</t>
+          <t>2,670</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2,284</t>
+          <t>2,844</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2,167</t>
+          <t>2,594</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>162,46K</t>
+          <t>416,53K</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>-6,56%</t>
+          <t>-3,84%</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>45485</v>
+        <v>45459</v>
       </c>
       <c r="B10" t="n">
-        <v>2.331</v>
+        <v>2.705</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2,287</t>
+          <t>2,846</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2,357</t>
+          <t>2,948</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2,252</t>
+          <t>2,672</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>101,06K</t>
+          <t>565,71K</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>2,15%</t>
+          <t>-6,11%</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>45484</v>
+        <v>45452</v>
       </c>
       <c r="B11" t="n">
-        <v>2.282</v>
+        <v>2.881</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>2,339</t>
+          <t>2,980</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2,353</t>
+          <t>3,159</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2,277</t>
+          <t>2,862</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>100,06K</t>
+          <t>1,09M</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>-2,69%</t>
+          <t>-1,27%</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>45483</v>
+        <v>45445</v>
       </c>
       <c r="B12" t="n">
-        <v>2.345</v>
+        <v>2.918</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>2,366</t>
+          <t>2,645</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2,396</t>
+          <t>2,967</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2,313</t>
+          <t>2,573</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>107,30K</t>
+          <t>1,06M</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>-0,64%</t>
+          <t>12,79%</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>45482</v>
+        <v>45438</v>
       </c>
       <c r="B13" t="n">
-        <v>2.36</v>
+        <v>2.587</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>2,384</t>
+          <t>2,503</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2,454</t>
+          <t>2,682</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2,351</t>
+          <t>2,417</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>106,05K</t>
+          <t>387,87K</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>-0,92%</t>
+          <t>2,66%</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>45481</v>
+        <v>45431</v>
       </c>
       <c r="B14" t="n">
-        <v>2.382</v>
+        <v>2.52</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>2,300</t>
+          <t>2,659</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>2,417</t>
+          <t>2,924</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2,300</t>
+          <t>2,493</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>126,72K</t>
+          <t>738,74K</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>1,36%</t>
+          <t>-4,04%</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>45478</v>
+        <v>45424</v>
       </c>
       <c r="B15" t="n">
-        <v>2.35</v>
+        <v>2.626</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>2,459</t>
+          <t>2,250</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>2,466</t>
+          <t>2,654</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2,347</t>
+          <t>2,214</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>98,43K</t>
+          <t>908,42K</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>-0,89%</t>
+          <t>16,61%</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>45477</v>
+        <v>45417</v>
       </c>
       <c r="B16" t="n">
-        <v>2.371</v>
+        <v>2.252</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>2,431</t>
+          <t>2,170</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>2,439</t>
+          <t>2,344</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2,335</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr"/>
+          <t>2,133</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>846,39K</t>
+        </is>
+      </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>-3,11%</t>
+          <t>5,14%</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>45476</v>
+        <v>45410</v>
       </c>
       <c r="B17" t="n">
-        <v>2.447</v>
+        <v>2.142</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>2,485</t>
+          <t>1,923</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>2,503</t>
+          <t>2,160</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2,434</t>
+          <t>1,913</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>70,97K</t>
+          <t>808,34K</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>-0,29%</t>
+          <t>32,71%</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>45475</v>
+        <v>45403</v>
       </c>
       <c r="B18" t="n">
-        <v>2.454</v>
+        <v>1.614</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>2,482</t>
+          <t>1,765</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>2,497</t>
+          <t>1,848</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2,436</t>
+          <t>1,482</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>96,17K</t>
+          <t>317,15K</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>-1,52%</t>
+          <t>-7,88%</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>45474</v>
+        <v>45396</v>
       </c>
       <c r="B19" t="n">
-        <v>2.492</v>
+        <v>1.752</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>2,581</t>
+          <t>1,772</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>2,599</t>
+          <t>1,806</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2,474</t>
+          <t>1,649</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>107,00K</t>
+          <t>869,31K</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>-4,08%</t>
+          <t>-1,02%</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>45471</v>
+        <v>45389</v>
       </c>
       <c r="B20" t="n">
-        <v>2.598</v>
+        <v>1.77</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>2,694</t>
+          <t>1,770</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>2,749</t>
+          <t>1,943</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>2,591</t>
+          <t>1,731</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>80,15K</t>
+          <t>999,32K</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>-2,88%</t>
+          <t>-11,94%</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>45470</v>
+        <v>45382</v>
       </c>
       <c r="B21" t="n">
-        <v>2.675</v>
+        <v>2.01</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>2,725</t>
+          <t>1,999</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>2,773</t>
+          <t>2,136</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2,665</t>
+          <t>1,958</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>61,99K</t>
+          <t>360,18K</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>-2,55%</t>
+          <t>14,01%</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>45469</v>
+        <v>45375</v>
       </c>
       <c r="B22" t="n">
-        <v>2.745</v>
+        <v>1.763</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>2,850</t>
+          <t>1,664</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>2,863</t>
+          <t>1,789</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2,731</t>
+          <t>1,481</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>141,35K</t>
+          <t>388,78K</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>-4,12%</t>
+          <t>6,27%</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>45468</v>
+        <v>45368</v>
       </c>
       <c r="B23" t="n">
-        <v>2.863</v>
+        <v>1.659</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>2,943</t>
+          <t>1,689</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>2,951</t>
+          <t>1,769</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2,831</t>
+          <t>1,647</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>158,42K</t>
+          <t>502,70K</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>-2,88%</t>
+          <t>0,24%</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
-        <v>45467</v>
+        <v>45361</v>
       </c>
       <c r="B24" t="n">
-        <v>2.948</v>
+        <v>1.655</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>2,813</t>
+          <t>1,805</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>2,953</t>
+          <t>1,841</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2,780</t>
+          <t>1,643</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>139,60K</t>
+          <t>859,05K</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>8,98%</t>
+          <t>-8,31%</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>45464</v>
+        <v>45354</v>
       </c>
       <c r="B25" t="n">
-        <v>2.705</v>
+        <v>1.805</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>2,725</t>
+          <t>1,873</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>2,770</t>
+          <t>2,009</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2,672</t>
+          <t>1,755</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>79,37K</t>
+          <t>752,20K</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>-1,31%</t>
+          <t>-1,63%</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
-        <v>45463</v>
+        <v>45347</v>
       </c>
       <c r="B26" t="n">
-        <v>2.741</v>
+        <v>1.835</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>2,903</t>
+          <t>1,660</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>2,948</t>
+          <t>1,918</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>2,723</t>
+          <t>1,511</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>186,69K</t>
+          <t>510,75K</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>-6,00%</t>
+          <t>14,47%</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
-        <v>45462</v>
+        <v>45340</v>
       </c>
       <c r="B27" t="n">
-        <v>2.916</v>
+        <v>1.603</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>2,904</t>
+          <t>1,533</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>2,928</t>
+          <t>1,792</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>2,859</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr"/>
+          <t>1,522</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>507,52K</t>
+        </is>
+      </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>0,24%</t>
+          <t>-0,37%</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
-        <v>45461</v>
+        <v>45333</v>
       </c>
       <c r="B28" t="n">
-        <v>2.909</v>
+        <v>1.609</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>2,772</t>
+          <t>1,805</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>2,916</t>
+          <t>1,863</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>2,772</t>
+          <t>1,573</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>147,41K</t>
+          <t>1,09M</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>4,34%</t>
+          <t>-12,89%</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
-        <v>45460</v>
+        <v>45326</v>
       </c>
       <c r="B29" t="n">
-        <v>2.788</v>
+        <v>1.847</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>2,846</t>
+          <t>2,110</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>2,848</t>
+          <t>2,127</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>2,759</t>
+          <t>1,817</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>152,24K</t>
+          <t>962,26K</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>-5,91%</t>
+          <t>-11,16%</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
-        <v>45457</v>
+        <v>45319</v>
       </c>
       <c r="B30" t="n">
-        <v>2.963</v>
+        <v>2.079</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>3,000</t>
+          <t>2,680</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>3,068</t>
+          <t>2,760</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>2,950</t>
+          <t>2,021</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>80,26K</t>
+          <t>447,53K</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>-2,44%</t>
+          <t>-23,34%</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
-        <v>45456</v>
+        <v>45312</v>
       </c>
       <c r="B31" t="n">
-        <v>3.037</v>
+        <v>2.712</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>3,104</t>
+          <t>2,380</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>3,167</t>
+          <t>2,884</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>2,978</t>
+          <t>2,311</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>94,27K</t>
+          <t>301,22K</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>-2,72%</t>
+          <t>7,66%</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
-        <v>45455</v>
+        <v>45305</v>
       </c>
       <c r="B32" t="n">
-        <v>3.122</v>
+        <v>2.519</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>3,194</t>
+          <t>3,113</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>3,194</t>
+          <t>3,189</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>3,073</t>
+          <t>2,514</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>101,31K</t>
+          <t>530,31K</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>-2,22%</t>
+          <t>-23,97%</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
-        <v>45454</v>
+        <v>45298</v>
       </c>
       <c r="B33" t="n">
-        <v>3.193</v>
+        <v>3.313</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>3,046</t>
+          <t>2,950</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>3,221</t>
+          <t>3,392</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>3,031</t>
+          <t>2,694</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>85,32K</t>
+          <t>1,08M</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>7,26%</t>
+          <t>14,52%</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
-        <v>45453</v>
+        <v>45291</v>
       </c>
       <c r="B34" t="n">
-        <v>2.977</v>
+        <v>2.893</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>3,055</t>
+          <t>2,605</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>3,163</t>
+          <t>2,906</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>2,945</t>
+          <t>2,524</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>106,18K</t>
+          <t>505,24K</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>-0,63%</t>
+          <t>15,08%</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="2" t="n">
-        <v>45450</v>
+        <v>45284</v>
       </c>
       <c r="B35" t="n">
-        <v>2.996</v>
+        <v>2.514</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>2,883</t>
+          <t>2,545</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>3,037</t>
+          <t>2,722</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>2,871</t>
+          <t>2,412</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>93,24K</t>
+          <t>170,75K</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>3,60%</t>
+          <t>-3,68%</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="n">
-        <v>45449</v>
+        <v>45277</v>
       </c>
       <c r="B36" t="n">
-        <v>2.892</v>
+        <v>2.61</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>2,829</t>
+          <t>2,503</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>2,946</t>
+          <t>2,620</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>2,796</t>
+          <t>2,385</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>73,60K</t>
+          <t>534,54K</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>2,26%</t>
+          <t>4,78%</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="2" t="n">
-        <v>45448</v>
+        <v>45270</v>
       </c>
       <c r="B37" t="n">
-        <v>2.828</v>
+        <v>2.491</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>2,694</t>
+          <t>2,490</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>2,854</t>
+          <t>2,544</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>2,681</t>
+          <t>2,235</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>76,26K</t>
+          <t>968,43K</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>5,92%</t>
+          <t>-3,49%</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="2" t="n">
-        <v>45447</v>
+        <v>45263</v>
       </c>
       <c r="B38" t="n">
-        <v>2.67</v>
+        <v>2.581</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>2,814</t>
+          <t>2,728</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>2,874</t>
+          <t>2,786</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>2,656</t>
+          <t>2,489</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>87,22K</t>
+          <t>748,53K</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>-4,78%</t>
+          <t>-8,28%</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="2" t="n">
-        <v>45446</v>
+        <v>45256</v>
       </c>
       <c r="B39" t="n">
-        <v>2.804</v>
+        <v>2.814</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>2,716</t>
+          <t>2,778</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>2,850</t>
+          <t>2,870</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>2,688</t>
+          <t>2,669</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>99,26K</t>
+          <t>360,52K</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>8,39%</t>
+          <t>-1,44%</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="2" t="n">
-        <v>45443</v>
+        <v>45249</v>
       </c>
       <c r="B40" t="n">
-        <v>2.587</v>
+        <v>2.855</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>2,570</t>
+          <t>2,957</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>2,624</t>
+          <t>2,958</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>2,518</t>
+          <t>2,798</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>139,12K</t>
+          <t>310,72K</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>0,58%</t>
+          <t>-3,55%</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="2" t="n">
-        <v>45442</v>
+        <v>45242</v>
       </c>
       <c r="B41" t="n">
-        <v>2.572</v>
+        <v>2.96</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>2,662</t>
+          <t>3,064</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>2,682</t>
+          <t>3,275</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>2,562</t>
+          <t>2,893</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>160,06K</t>
+          <t>805,56K</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>3,17%</t>
+          <t>-2,41%</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="2" t="n">
-        <v>45441</v>
+        <v>45235</v>
       </c>
       <c r="B42" t="n">
-        <v>2.493</v>
+        <v>3.033</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>2,594</t>
+          <t>3,373</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>2,669</t>
+          <t>3,407</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>2,417</t>
+          <t>2,989</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>2,66K</t>
+          <t>687,25K</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>-3,75%</t>
+          <t>-13,71%</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="2" t="n">
-        <v>45440</v>
+        <v>45228</v>
       </c>
       <c r="B43" t="n">
-        <v>2.59</v>
+        <v>3.515</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>2,503</t>
+          <t>3,400</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>2,621</t>
+          <t>3,630</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>2,475</t>
+          <t>3,318</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>86,03K</t>
+          <t>627,63K</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>-6,83%</t>
+          <t>11,09%</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="2" t="n">
-        <v>45439</v>
+        <v>45221</v>
       </c>
       <c r="B44" t="n">
-        <v>2.78</v>
+        <v>3.164</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>2,747</t>
+          <t>2,905</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>2,853</t>
+          <t>3,401</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>2,742</t>
-        </is>
-      </c>
-      <c r="F44" t="inlineStr"/>
+          <t>2,861</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>284,63K</t>
+        </is>
+      </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>1,16%</t>
+          <t>9,14%</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="2" t="n">
-        <v>45438</v>
+        <v>45214</v>
       </c>
       <c r="B45" t="n">
-        <v>2.748</v>
+        <v>2.899</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>2,747</t>
+          <t>3,185</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>2,760</t>
+          <t>3,185</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>2,732</t>
-        </is>
-      </c>
-      <c r="F45" t="inlineStr"/>
+          <t>2,880</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>560,11K</t>
+        </is>
+      </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>9,05%</t>
+          <t>-10,41%</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="2" t="n">
-        <v>45436</v>
+        <v>45207</v>
       </c>
       <c r="B46" t="n">
-        <v>2.52</v>
+        <v>3.236</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>2,676</t>
+          <t>3,350</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>2,709</t>
+          <t>3,471</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>2,493</t>
+          <t>3,203</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>51,81K</t>
+          <t>750,13K</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>-5,16%</t>
+          <t>-3,06%</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="2" t="n">
-        <v>45435</v>
+        <v>45200</v>
       </c>
       <c r="B47" t="n">
-        <v>2.657</v>
+        <v>3.338</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>2,799</t>
+          <t>2,958</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>2,924</t>
+          <t>3,364</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>2,640</t>
+          <t>2,820</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>116,69K</t>
+          <t>628,89K</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>-6,51%</t>
+          <t>13,96%</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="2" t="n">
-        <v>45434</v>
+        <v>45193</v>
       </c>
       <c r="B48" t="n">
-        <v>2.842</v>
+        <v>2.929</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>2,665</t>
+          <t>2,657</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>2,851</t>
+          <t>2,997</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>2,609</t>
+          <t>2,552</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>184,82K</t>
+          <t>218,82K</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>6,40%</t>
+          <t>11,07%</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="2" t="n">
-        <v>45433</v>
+        <v>45186</v>
       </c>
       <c r="B49" t="n">
-        <v>2.671</v>
+        <v>2.637</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>2,733</t>
+          <t>2,624</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>2,798</t>
+          <t>2,872</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>2,640</t>
+          <t>2,595</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>174,16K</t>
+          <t>533,39K</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>-2,91%</t>
+          <t>-0,26%</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="2" t="n">
-        <v>45432</v>
+        <v>45179</v>
       </c>
       <c r="B50" t="n">
-        <v>2.751</v>
+        <v>2.644</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>2,659</t>
+          <t>2,610</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>2,756</t>
+          <t>2,823</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>2,625</t>
+          <t>2,541</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>211,26K</t>
+          <t>658,86K</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>4,76%</t>
+          <t>1,50%</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="2" t="n">
-        <v>45429</v>
+        <v>45172</v>
       </c>
       <c r="B51" t="n">
-        <v>2.626</v>
+        <v>2.605</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>2,487</t>
+          <t>2,700</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>2,654</t>
+          <t>2,708</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>2,485</t>
+          <t>2,500</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>185,80K</t>
+          <t>435,33K</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>5,25%</t>
+          <t>-5,79%</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="2" t="n">
-        <v>45428</v>
+        <v>45165</v>
       </c>
       <c r="B52" t="n">
-        <v>2.495</v>
+        <v>2.765</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>2,405</t>
+          <t>2,635</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>2,575</t>
+          <t>2,865</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>2,389</t>
+          <t>2,515</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>229,62K</t>
+          <t>383,46K</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>3,27%</t>
+          <t>8,86%</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="2" t="n">
-        <v>45427</v>
+        <v>45158</v>
       </c>
       <c r="B53" t="n">
-        <v>2.416</v>
+        <v>2.54</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>2,343</t>
+          <t>2,560</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>2,424</t>
+          <t>2,660</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>2,313</t>
+          <t>2,425</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>180,74K</t>
+          <t>384,52K</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>3,07%</t>
+          <t>-0,43%</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="2" t="n">
-        <v>45426</v>
+        <v>45151</v>
       </c>
       <c r="B54" t="n">
-        <v>2.344</v>
+        <v>2.551</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>2,362</t>
+          <t>2,776</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>2,397</t>
+          <t>2,863</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>2,306</t>
+          <t>2,524</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>147,57K</t>
+          <t>514,45K</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>-1,55%</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" s="2" t="n">
-        <v>45425</v>
-      </c>
-      <c r="B55" t="n">
-        <v>2.381</v>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>2,250</t>
-        </is>
-      </c>
-      <c r="D55" t="inlineStr">
-        <is>
-          <t>2,384</t>
-        </is>
-      </c>
-      <c r="E55" t="inlineStr">
-        <is>
-          <t>2,214</t>
-        </is>
-      </c>
-      <c r="F55" t="inlineStr">
-        <is>
-          <t>164,69K</t>
-        </is>
-      </c>
-      <c r="G55" t="inlineStr">
-        <is>
-          <t>5,73%</t>
-        </is>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" s="2" t="n">
-        <v>45422</v>
-      </c>
-      <c r="B56" t="n">
-        <v>2.252</v>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>2,307</t>
-        </is>
-      </c>
-      <c r="D56" t="inlineStr">
-        <is>
-          <t>2,344</t>
-        </is>
-      </c>
-      <c r="E56" t="inlineStr">
-        <is>
-          <t>2,242</t>
-        </is>
-      </c>
-      <c r="F56" t="inlineStr">
-        <is>
-          <t>142,99K</t>
-        </is>
-      </c>
-      <c r="G56" t="inlineStr">
-        <is>
-          <t>-2,13%</t>
-        </is>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" s="2" t="n">
-        <v>45421</v>
-      </c>
-      <c r="B57" t="n">
-        <v>2.301</v>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>2,186</t>
-        </is>
-      </c>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>2,316</t>
-        </is>
-      </c>
-      <c r="E57" t="inlineStr">
-        <is>
-          <t>2,153</t>
-        </is>
-      </c>
-      <c r="F57" t="inlineStr">
-        <is>
-          <t>207,68K</t>
-        </is>
-      </c>
-      <c r="G57" t="inlineStr">
-        <is>
-          <t>5,21%</t>
-        </is>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" s="2" t="n">
-        <v>45420</v>
-      </c>
-      <c r="B58" t="n">
-        <v>2.187</v>
-      </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>2,219</t>
-        </is>
-      </c>
-      <c r="D58" t="inlineStr">
-        <is>
-          <t>2,274</t>
-        </is>
-      </c>
-      <c r="E58" t="inlineStr">
-        <is>
-          <t>2,167</t>
-        </is>
-      </c>
-      <c r="F58" t="inlineStr">
-        <is>
-          <t>149,91K</t>
-        </is>
-      </c>
-      <c r="G58" t="inlineStr">
-        <is>
-          <t>-0,91%</t>
-        </is>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" s="2" t="n">
-        <v>45419</v>
-      </c>
-      <c r="B59" t="n">
-        <v>2.207</v>
-      </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>2,206</t>
-        </is>
-      </c>
-      <c r="D59" t="inlineStr">
-        <is>
-          <t>2,230</t>
-        </is>
-      </c>
-      <c r="E59" t="inlineStr">
-        <is>
-          <t>2,142</t>
-        </is>
-      </c>
-      <c r="F59" t="inlineStr">
-        <is>
-          <t>149,43K</t>
-        </is>
-      </c>
-      <c r="G59" t="inlineStr">
-        <is>
-          <t>0,55%</t>
-        </is>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" s="2" t="n">
-        <v>45418</v>
-      </c>
-      <c r="B60" t="n">
-        <v>2.195</v>
-      </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>2,170</t>
-        </is>
-      </c>
-      <c r="D60" t="inlineStr">
-        <is>
-          <t>2,262</t>
-        </is>
-      </c>
-      <c r="E60" t="inlineStr">
-        <is>
-          <t>2,133</t>
-        </is>
-      </c>
-      <c r="F60" t="inlineStr">
-        <is>
-          <t>196,38K</t>
-        </is>
-      </c>
-      <c r="G60" t="inlineStr">
-        <is>
-          <t>2,47%</t>
-        </is>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" s="2" t="n">
-        <v>45415</v>
-      </c>
-      <c r="B61" t="n">
-        <v>2.142</v>
-      </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>2,031</t>
-        </is>
-      </c>
-      <c r="D61" t="inlineStr">
-        <is>
-          <t>2,160</t>
-        </is>
-      </c>
-      <c r="E61" t="inlineStr">
-        <is>
-          <t>2,012</t>
-        </is>
-      </c>
-      <c r="F61" t="inlineStr">
-        <is>
-          <t>209,46K</t>
-        </is>
-      </c>
-      <c r="G61" t="inlineStr">
-        <is>
-          <t>5,26%</t>
-        </is>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" s="2" t="n">
-        <v>45414</v>
-      </c>
-      <c r="B62" t="n">
-        <v>2.035</v>
-      </c>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t>1,931</t>
-        </is>
-      </c>
-      <c r="D62" t="inlineStr">
-        <is>
-          <t>2,050</t>
-        </is>
-      </c>
-      <c r="E62" t="inlineStr">
-        <is>
-          <t>1,927</t>
-        </is>
-      </c>
-      <c r="F62" t="inlineStr">
-        <is>
-          <t>153,74K</t>
-        </is>
-      </c>
-      <c r="G62" t="inlineStr">
-        <is>
-          <t>5,33%</t>
-        </is>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" s="2" t="n">
-        <v>45413</v>
-      </c>
-      <c r="B63" t="n">
-        <v>1.932</v>
-      </c>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t>1,954</t>
-        </is>
-      </c>
-      <c r="D63" t="inlineStr">
-        <is>
-          <t>1,970</t>
-        </is>
-      </c>
-      <c r="E63" t="inlineStr">
-        <is>
-          <t>1,913</t>
-        </is>
-      </c>
-      <c r="F63" t="inlineStr">
-        <is>
-          <t>135,92K</t>
-        </is>
-      </c>
-      <c r="G63" t="inlineStr">
-        <is>
-          <t>-2,96%</t>
-        </is>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" s="2" t="n">
-        <v>45412</v>
-      </c>
-      <c r="B64" t="n">
-        <v>1.991</v>
-      </c>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t>2,050</t>
-        </is>
-      </c>
-      <c r="D64" t="inlineStr">
-        <is>
-          <t>2,092</t>
-        </is>
-      </c>
-      <c r="E64" t="inlineStr">
-        <is>
-          <t>1,951</t>
-        </is>
-      </c>
-      <c r="F64" t="inlineStr">
-        <is>
-          <t>150,37K</t>
-        </is>
-      </c>
-      <c r="G64" t="inlineStr">
-        <is>
-          <t>-1,92%</t>
-        </is>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" s="2" t="n">
-        <v>45411</v>
-      </c>
-      <c r="B65" t="n">
-        <v>2.03</v>
-      </c>
-      <c r="C65" t="inlineStr">
-        <is>
-          <t>1,923</t>
-        </is>
-      </c>
-      <c r="D65" t="inlineStr">
-        <is>
-          <t>2,056</t>
-        </is>
-      </c>
-      <c r="E65" t="inlineStr">
-        <is>
-          <t>1,916</t>
-        </is>
-      </c>
-      <c r="F65" t="inlineStr">
-        <is>
-          <t>158,86K</t>
-        </is>
-      </c>
-      <c r="G65" t="inlineStr">
-        <is>
-          <t>25,77%</t>
-        </is>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" s="2" t="n">
-        <v>45408</v>
-      </c>
-      <c r="B66" t="n">
-        <v>1.614</v>
-      </c>
-      <c r="C66" t="inlineStr">
-        <is>
-          <t>1,622</t>
-        </is>
-      </c>
-      <c r="D66" t="inlineStr">
-        <is>
-          <t>1,628</t>
-        </is>
-      </c>
-      <c r="E66" t="inlineStr">
-        <is>
-          <t>1,482</t>
-        </is>
-      </c>
-      <c r="F66" t="inlineStr">
-        <is>
-          <t>4,93K</t>
-        </is>
-      </c>
-      <c r="G66" t="inlineStr">
-        <is>
-          <t>-1,47%</t>
-        </is>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" s="2" t="n">
-        <v>45407</v>
-      </c>
-      <c r="B67" t="n">
-        <v>1.638</v>
-      </c>
-      <c r="C67" t="inlineStr">
-        <is>
-          <t>1,644</t>
-        </is>
-      </c>
-      <c r="D67" t="inlineStr">
-        <is>
-          <t>1,675</t>
-        </is>
-      </c>
-      <c r="E67" t="inlineStr">
-        <is>
-          <t>1,583</t>
-        </is>
-      </c>
-      <c r="F67" t="inlineStr">
-        <is>
-          <t>75,48K</t>
-        </is>
-      </c>
-      <c r="G67" t="inlineStr">
-        <is>
-          <t>-0,91%</t>
-        </is>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" s="2" t="n">
-        <v>45406</v>
-      </c>
-      <c r="B68" t="n">
-        <v>1.653</v>
-      </c>
-      <c r="C68" t="inlineStr">
-        <is>
-          <t>1,836</t>
-        </is>
-      </c>
-      <c r="D68" t="inlineStr">
-        <is>
-          <t>1,840</t>
-        </is>
-      </c>
-      <c r="E68" t="inlineStr">
-        <is>
-          <t>1,634</t>
-        </is>
-      </c>
-      <c r="F68" t="inlineStr">
-        <is>
-          <t>58,15K</t>
-        </is>
-      </c>
-      <c r="G68" t="inlineStr">
-        <is>
-          <t>-8,77%</t>
+          <t>-7,91%</t>
         </is>
       </c>
     </row>

</xml_diff>